<commit_message>
Added Components to Power Consumption and Cables for purchase
</commit_message>
<xml_diff>
--- a/SB_Power_Consumption.xlsx
+++ b/SB_Power_Consumption.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My Files\GenInfy\PCB Designs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My Files\GenInfy\PCB Designs\SB_Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{39D515E4-7548-4A78-AA59-AFA62B9DC41D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA0F06D-A2DE-48CC-8B90-DD88826255FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7305" windowWidth="29040" windowHeight="15840" xr2:uid="{62672528-1BFE-4DBF-8B13-7FC9E250EFAF}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="100">
   <si>
     <t>Section E</t>
   </si>
@@ -105,9 +105,6 @@
     <t>0.2A</t>
   </si>
   <si>
-    <t>Pump</t>
-  </si>
-  <si>
     <t>5v</t>
   </si>
   <si>
@@ -156,9 +153,6 @@
     <t>0.53A</t>
   </si>
   <si>
-    <t>4.52A</t>
-  </si>
-  <si>
     <t>Motor Driver</t>
   </si>
   <si>
@@ -213,13 +207,7 @@
     <t>Nema</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>Buzzer</t>
-  </si>
-  <si>
-    <t>LED</t>
   </si>
   <si>
     <t>Display Fan 1</t>
@@ -317,12 +305,117 @@
   <si>
     <t>Maximum</t>
   </si>
+  <si>
+    <t>2.3A</t>
+  </si>
+  <si>
+    <t>4.5A</t>
+  </si>
+  <si>
+    <t>10A</t>
+  </si>
+  <si>
+    <t>LED x 3</t>
+  </si>
+  <si>
+    <t>0.75A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temperature Sensor </t>
+  </si>
+  <si>
+    <t>Datasheets</t>
+  </si>
+  <si>
+    <t>https://datasheets.maximintegrated.com/en/ds/DS18B20.pdf</t>
+  </si>
+  <si>
+    <t>Water Pump</t>
+  </si>
+  <si>
+    <t>Servo</t>
+  </si>
+  <si>
+    <t>Solenoid Valve</t>
+  </si>
+  <si>
+    <t>Fan</t>
+  </si>
+  <si>
+    <t>4.40A</t>
+  </si>
+  <si>
+    <t>https://sofasco.com/pages/sd2010-series-dc-cooling-fan</t>
+  </si>
+  <si>
+    <t>CC Motor</t>
+  </si>
+  <si>
+    <t>https://www.alibaba.com/product-detail/3-V-6-Volt-12V-Electric_60776760546.html?spm=a2700.wholesale.deiletai6.22.725b43ce9JV9NR</t>
+  </si>
+  <si>
+    <t>http://www.towerpro.com.tw/product/mg995-robot-servo-360-180-rotation/</t>
+  </si>
+  <si>
+    <t>https://robokits.co.in/automation-control-cnc/spindle-motor-for-cnc-with-drive/vfd-and-drive-for-spindle-motors/cnc-spindle-300w-er11-air-cooled-48v-12000rpm-for-engraving-with-universal-motor-controller-with-pwm-speed-control-switch</t>
+  </si>
+  <si>
+    <t>https://www.waveshare.com/5inch-hdmi-lcd.htm</t>
+  </si>
+  <si>
+    <t>https://www.omc-stepperonline.com/nema-14-stepper-motor/Dual-Shaft-Nema-14-18deg-18Ncm-2556ozin-08A-54V-352x352x34mm-4-Wires.html</t>
+  </si>
+  <si>
+    <t>https://www.pololu.com/category/60/micro-metal-gearmotors</t>
+  </si>
+  <si>
+    <t>Couldn't get manufacturer info</t>
+  </si>
+  <si>
+    <t>8.9A</t>
+  </si>
+  <si>
+    <t>1.48A</t>
+  </si>
+  <si>
+    <t>3.45A</t>
+  </si>
+  <si>
+    <t>10.5A</t>
+  </si>
+  <si>
+    <t>TB6612FNG</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/14451</t>
+  </si>
+  <si>
+    <t>Pyboard</t>
+  </si>
+  <si>
+    <t>Pyboard v1.1</t>
+  </si>
+  <si>
+    <t>https://docs.micropython.org/en/latest/pyboard/quickref.html</t>
+  </si>
+  <si>
+    <t>Refer Datasheet</t>
+  </si>
+  <si>
+    <t>SmartElex 15S DC Motor Driver</t>
+  </si>
+  <si>
+    <t>Grinding Motor Driver</t>
+  </si>
+  <si>
+    <t>https://robu.in/product/smartelex-15s-dc-motor-driver-13a-30a-peak/#tab-product_download_66939_tab</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -350,6 +443,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -368,14 +469,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -688,10 +792,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6620B2B8-7A56-4734-9209-8A07EC7E77FB}">
-  <dimension ref="A1:D77"/>
+  <dimension ref="A1:D91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="C92" sqref="C92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -721,7 +825,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -735,7 +839,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
@@ -749,7 +853,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
@@ -780,10 +884,10 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="D7" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -794,10 +898,10 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -808,10 +912,24 @@
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="D9" t="s">
-        <v>55</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -825,6 +943,14 @@
         <v>18</v>
       </c>
     </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" t="s">
+        <v>65</v>
+      </c>
+    </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>10</v>
@@ -919,13 +1045,13 @@
         <v>7</v>
       </c>
       <c r="B21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" t="s">
         <v>26</v>
-      </c>
-      <c r="C21" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -933,13 +1059,13 @@
         <v>8</v>
       </c>
       <c r="B22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C22" t="s">
         <v>6</v>
       </c>
       <c r="D22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -947,13 +1073,13 @@
         <v>9</v>
       </c>
       <c r="B23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C23" t="s">
         <v>6</v>
       </c>
       <c r="D23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -961,13 +1087,13 @@
         <v>10</v>
       </c>
       <c r="B24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" t="s">
         <v>19</v>
       </c>
-      <c r="C24" t="s">
-        <v>20</v>
-      </c>
       <c r="D24" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -978,10 +1104,10 @@
         <v>22</v>
       </c>
       <c r="C25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -992,10 +1118,10 @@
         <v>23</v>
       </c>
       <c r="C26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -1003,13 +1129,13 @@
         <v>13</v>
       </c>
       <c r="B27" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C27" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="D27" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -1020,10 +1146,10 @@
         <v>30</v>
       </c>
       <c r="C28" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="D28" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -1031,45 +1157,45 @@
         <v>15</v>
       </c>
       <c r="B29" t="s">
-        <v>31</v>
+        <v>93</v>
       </c>
       <c r="C29" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="D29" t="s">
-        <v>33</v>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B30" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B31" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="C31" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="D31" t="s">
-        <v>35</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C32" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="D32" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C33" t="s">
-        <v>32</v>
-      </c>
-      <c r="D33" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -1077,7 +1203,7 @@
         <v>1</v>
       </c>
       <c r="B36" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C36" t="s">
         <v>6</v>
@@ -1091,7 +1217,7 @@
         <v>2</v>
       </c>
       <c r="B37" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C37" t="s">
         <v>6</v>
@@ -1105,13 +1231,13 @@
         <v>3</v>
       </c>
       <c r="B38" t="s">
+        <v>38</v>
+      </c>
+      <c r="C38" t="s">
+        <v>39</v>
+      </c>
+      <c r="D38" t="s">
         <v>40</v>
-      </c>
-      <c r="C38" t="s">
-        <v>41</v>
-      </c>
-      <c r="D38" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
@@ -1119,13 +1245,13 @@
         <v>4</v>
       </c>
       <c r="B39" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C39" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D39" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -1133,13 +1259,13 @@
         <v>5</v>
       </c>
       <c r="B40" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C40" t="s">
         <v>6</v>
       </c>
       <c r="D40" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
@@ -1147,13 +1273,27 @@
         <v>6</v>
       </c>
       <c r="B41" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C41" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D41" t="s">
-        <v>55</v>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>7</v>
+      </c>
+      <c r="B42" t="s">
+        <v>97</v>
+      </c>
+      <c r="C42" t="s">
+        <v>31</v>
+      </c>
+      <c r="D42" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
@@ -1169,23 +1309,23 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C44" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D44" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C45" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D45" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
@@ -1193,13 +1333,13 @@
         <v>1</v>
       </c>
       <c r="B48" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C48" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D48" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
@@ -1207,13 +1347,13 @@
         <v>2</v>
       </c>
       <c r="B49" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C49" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D49" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
@@ -1221,7 +1361,7 @@
         <v>3</v>
       </c>
       <c r="B50" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C50" t="s">
         <v>6</v>
@@ -1235,91 +1375,91 @@
         <v>4</v>
       </c>
       <c r="B51" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="C51" t="s">
-        <v>55</v>
+        <v>6</v>
       </c>
       <c r="D51" t="s">
-        <v>55</v>
+        <v>20</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B52" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="C52" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="D52" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B53" t="s">
         <v>54</v>
       </c>
       <c r="C53" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="D53" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B54" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C54" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="D54" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B55" t="s">
-        <v>58</v>
+        <v>29</v>
       </c>
       <c r="C55" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="D55" t="s">
-        <v>55</v>
+        <v>4</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B56" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C56" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="D56" t="s">
-        <v>55</v>
+        <v>4</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B57" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="C57" t="s">
         <v>6</v>
@@ -1330,169 +1470,269 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B58" t="s">
+        <v>58</v>
+      </c>
+      <c r="C58" t="s">
+        <v>6</v>
+      </c>
+      <c r="D58" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B60" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C60" t="s">
+        <v>6</v>
+      </c>
+      <c r="D60" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C61" t="s">
+        <v>19</v>
+      </c>
+      <c r="D61" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C58" t="s">
-        <v>6</v>
-      </c>
-      <c r="D58" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59">
-        <v>12</v>
-      </c>
-      <c r="B59" t="s">
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>1</v>
+      </c>
+      <c r="B64" t="s">
+        <v>62</v>
+      </c>
+      <c r="C64" t="s">
+        <v>6</v>
+      </c>
+      <c r="D64" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>2</v>
+      </c>
+      <c r="B65" t="s">
         <v>61</v>
       </c>
-      <c r="C59" t="s">
-        <v>6</v>
-      </c>
-      <c r="D59" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60">
-        <v>13</v>
-      </c>
-      <c r="B60" t="s">
-        <v>62</v>
-      </c>
-      <c r="C60" t="s">
-        <v>6</v>
-      </c>
-      <c r="D60" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B62" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C62" t="s">
-        <v>6</v>
-      </c>
-      <c r="D62" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C63" t="s">
-        <v>20</v>
-      </c>
-      <c r="D63" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="1" t="s">
-        <v>64</v>
+      <c r="C65" t="s">
+        <v>6</v>
+      </c>
+      <c r="D65" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B66" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="C66" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="D66" t="s">
-        <v>4</v>
+        <v>69</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B67" t="s">
-        <v>65</v>
+        <v>91</v>
       </c>
       <c r="C67" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="D67" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68">
-        <v>3</v>
-      </c>
-      <c r="B68" t="s">
-        <v>46</v>
+      <c r="B68" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="C68" t="s">
-        <v>55</v>
+        <v>6</v>
       </c>
       <c r="D68" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B70" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C70" t="s">
-        <v>6</v>
-      </c>
-      <c r="D70" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C71" t="s">
-        <v>55</v>
-      </c>
-      <c r="D71" t="s">
-        <v>55</v>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C69" t="s">
+        <v>39</v>
+      </c>
+      <c r="D69" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B72" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C72" t="s">
+        <v>6</v>
+      </c>
+      <c r="D72" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C73" t="s">
+        <v>19</v>
+      </c>
+      <c r="D73" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B74" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="C74" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="D74" t="s">
-        <v>25</v>
+        <v>89</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C75" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="D75" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C76" t="s">
-        <v>41</v>
-      </c>
-      <c r="D76" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C77" t="s">
-        <v>32</v>
-      </c>
-      <c r="D77" t="s">
-        <v>55</v>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B79" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B80" t="s">
+        <v>70</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="81" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B81" t="s">
+        <v>73</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B82" t="s">
+        <v>74</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B83" t="s">
+        <v>75</v>
+      </c>
+      <c r="C83" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="84" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B84" t="s">
+        <v>76</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="85" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B85" t="s">
+        <v>44</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="86" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B86" t="s">
+        <v>47</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="87" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B87" t="s">
+        <v>52</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="88" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B88" t="s">
+        <v>79</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="89" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B89" t="s">
+        <v>91</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="90" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B90" t="s">
+        <v>94</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="91" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B91" t="s">
+        <v>98</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="C80" r:id="rId1" xr:uid="{F5BB1312-1EF1-4095-A57D-C28C2C46FAEE}"/>
+    <hyperlink ref="C84" r:id="rId2" xr:uid="{60819609-A8E1-4E1D-90C0-3568F139ED26}"/>
+    <hyperlink ref="C81" r:id="rId3" xr:uid="{941DB92D-C1FE-47D8-805F-2287ACB7B704}"/>
+    <hyperlink ref="C82" r:id="rId4" xr:uid="{CA8AA13D-4D80-49D7-891F-5C4F1E3DD98F}"/>
+    <hyperlink ref="C85" r:id="rId5" xr:uid="{F7834EE0-5AEF-438F-A50A-66823F273D6A}"/>
+    <hyperlink ref="C86" r:id="rId6" xr:uid="{14F5A7F8-E7F6-4900-8BF9-285B45690FFA}"/>
+    <hyperlink ref="C87" r:id="rId7" xr:uid="{8BA60238-20E4-46B8-9491-2F7697134A35}"/>
+    <hyperlink ref="C88" r:id="rId8" xr:uid="{CD5F6A81-523C-4475-A657-7CA7C84A44D4}"/>
+    <hyperlink ref="C89" r:id="rId9" xr:uid="{0434E14F-4A3E-4DB8-A4BE-95F70558DC31}"/>
+    <hyperlink ref="C90" r:id="rId10" xr:uid="{14097A58-CD0C-45CC-A5B9-EBDCA17245AE}"/>
+    <hyperlink ref="C91" r:id="rId11" location="tab-product_download_66939_tab" xr:uid="{21FD1A59-6F33-407E-B79F-70E22C0B47E3}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>